<commit_message>
Rebuild synchro pour AAPS et Xdrip
</commit_message>
<xml_diff>
--- a/Modèles.xlsx
+++ b/Modèles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="modèles" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="575">
   <si>
     <t>deviceId</t>
   </si>
@@ -1748,6 +1748,18 @@
   </si>
   <si>
     <t>pixel Y</t>
+  </si>
+  <si>
+    <t>AAPS</t>
+  </si>
+  <si>
+    <t>XDRIP</t>
+  </si>
+  <si>
+    <t>millis</t>
+  </si>
+  <si>
+    <t>secondes</t>
   </si>
 </sst>
 </file>
@@ -8981,7 +8993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -9099,67 +9111,67 @@
         <v>345</v>
       </c>
       <c r="I2" s="4">
-        <f>$C2*I$1</f>
+        <f t="shared" ref="I2:P14" si="0">$C2*I$1</f>
         <v>109</v>
       </c>
       <c r="J2" s="4">
-        <f>$C2*J$1</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="K2" s="4">
-        <f>$C2*K$1</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="L2" s="4">
-        <f>$C2*L$1</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="M2" s="4">
-        <f>$C2*M$1</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="N2" s="4">
-        <f>$C2*N$1</f>
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
       <c r="O2" s="4">
-        <f>$C2*O$1</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="P2" s="4">
-        <f>$C2*P$1</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="R2" s="4">
-        <f>$E2*R$1</f>
+        <f t="shared" ref="R2:Y14" si="1">$E2*R$1</f>
         <v>28.34</v>
       </c>
       <c r="S2" s="4">
-        <f>$E2*S$1</f>
+        <f t="shared" si="1"/>
         <v>31.200000000000003</v>
       </c>
       <c r="T2" s="4">
-        <f>$E2*T$1</f>
+        <f t="shared" si="1"/>
         <v>33.800000000000004</v>
       </c>
       <c r="U2" s="4">
-        <f>$E2*U$1</f>
+        <f t="shared" si="1"/>
         <v>36.4</v>
       </c>
       <c r="V2" s="4">
-        <f>$E2*V$1</f>
+        <f t="shared" si="1"/>
         <v>46.800000000000004</v>
       </c>
       <c r="W2" s="4">
-        <f>$E2*W$1</f>
+        <f t="shared" si="1"/>
         <v>50.7</v>
       </c>
       <c r="X2" s="4">
-        <f>$E2*X$1</f>
+        <f t="shared" si="1"/>
         <v>54.08</v>
       </c>
       <c r="Y2" s="4">
-        <f>$E2*Y$1</f>
+        <f t="shared" si="1"/>
         <v>59.02</v>
       </c>
       <c r="AB2" s="12" t="s">
@@ -9174,14 +9186,14 @@
         <v>208</v>
       </c>
       <c r="C3" s="25">
-        <f t="shared" ref="C3:E14" si="0">ROUND(B3/$A$1,2)</f>
+        <f t="shared" ref="C3:E14" si="2">ROUND(B3/$A$1,2)</f>
         <v>0.5</v>
       </c>
       <c r="D3" s="24">
         <v>131</v>
       </c>
       <c r="E3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.31</v>
       </c>
       <c r="F3" s="21" t="s">
@@ -9191,67 +9203,67 @@
         <v>345</v>
       </c>
       <c r="I3" s="4">
-        <f>$C3*I$1</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="J3" s="4">
-        <f>$C3*J$1</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="K3" s="4">
-        <f>$C3*K$1</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="L3" s="4">
-        <f>$C3*L$1</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="M3" s="4">
-        <f>$C3*M$1</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="N3" s="4">
-        <f>$C3*N$1</f>
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
       <c r="O3" s="4">
-        <f>$C3*O$1</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="P3" s="4">
-        <f>$C3*P$1</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="R3" s="4">
-        <f>$E3*R$1</f>
+        <f t="shared" si="1"/>
         <v>67.58</v>
       </c>
       <c r="S3" s="4">
-        <f>$E3*S$1</f>
+        <f t="shared" si="1"/>
         <v>74.400000000000006</v>
       </c>
       <c r="T3" s="4">
-        <f>$E3*T$1</f>
+        <f t="shared" si="1"/>
         <v>80.599999999999994</v>
       </c>
       <c r="U3" s="4">
-        <f>$E3*U$1</f>
+        <f t="shared" si="1"/>
         <v>86.8</v>
       </c>
       <c r="V3" s="4">
-        <f>$E3*V$1</f>
+        <f t="shared" si="1"/>
         <v>111.6</v>
       </c>
       <c r="W3" s="4">
-        <f>$E3*W$1</f>
+        <f t="shared" si="1"/>
         <v>120.9</v>
       </c>
       <c r="X3" s="4">
-        <f>$E3*X$1</f>
+        <f t="shared" si="1"/>
         <v>128.96</v>
       </c>
       <c r="Y3" s="4">
-        <f>$E3*Y$1</f>
+        <f t="shared" si="1"/>
         <v>140.74</v>
       </c>
       <c r="AB3" s="15" t="s">
@@ -9266,14 +9278,14 @@
         <v>50</v>
       </c>
       <c r="C4" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
       <c r="D4" s="24">
         <v>163</v>
       </c>
       <c r="E4" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.39</v>
       </c>
       <c r="F4" s="21" t="s">
@@ -9283,67 +9295,67 @@
         <v>345</v>
       </c>
       <c r="I4" s="4">
-        <f>$C4*I$1</f>
+        <f t="shared" si="0"/>
         <v>26.16</v>
       </c>
       <c r="J4" s="4">
-        <f>$C4*J$1</f>
+        <f t="shared" si="0"/>
         <v>28.799999999999997</v>
       </c>
       <c r="K4" s="4">
-        <f>$C4*K$1</f>
+        <f t="shared" si="0"/>
         <v>31.2</v>
       </c>
       <c r="L4" s="4">
-        <f>$C4*L$1</f>
+        <f t="shared" si="0"/>
         <v>33.6</v>
       </c>
       <c r="M4" s="4">
-        <f>$C4*M$1</f>
+        <f t="shared" si="0"/>
         <v>43.199999999999996</v>
       </c>
       <c r="N4" s="4">
-        <f>$C4*N$1</f>
+        <f t="shared" si="0"/>
         <v>46.8</v>
       </c>
       <c r="O4" s="4">
-        <f>$C4*O$1</f>
+        <f t="shared" si="0"/>
         <v>49.92</v>
       </c>
       <c r="P4" s="4">
-        <f>$C4*P$1</f>
+        <f t="shared" si="0"/>
         <v>54.48</v>
       </c>
       <c r="R4" s="4">
-        <f>$E4*R$1</f>
+        <f t="shared" si="1"/>
         <v>85.02</v>
       </c>
       <c r="S4" s="4">
-        <f>$E4*S$1</f>
+        <f t="shared" si="1"/>
         <v>93.600000000000009</v>
       </c>
       <c r="T4" s="4">
-        <f>$E4*T$1</f>
+        <f t="shared" si="1"/>
         <v>101.4</v>
       </c>
       <c r="U4" s="4">
-        <f>$E4*U$1</f>
+        <f t="shared" si="1"/>
         <v>109.2</v>
       </c>
       <c r="V4" s="4">
-        <f>$E4*V$1</f>
+        <f t="shared" si="1"/>
         <v>140.4</v>
       </c>
       <c r="W4" s="4">
-        <f>$E4*W$1</f>
+        <f t="shared" si="1"/>
         <v>152.1</v>
       </c>
       <c r="X4" s="4">
-        <f>$E4*X$1</f>
+        <f t="shared" si="1"/>
         <v>162.24</v>
       </c>
       <c r="Y4" s="4">
-        <f>$E4*Y$1</f>
+        <f t="shared" si="1"/>
         <v>177.06</v>
       </c>
     </row>
@@ -9355,14 +9367,14 @@
         <v>312</v>
       </c>
       <c r="C5" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
       <c r="D5" s="24">
         <v>242</v>
       </c>
       <c r="E5" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.57999999999999996</v>
       </c>
       <c r="F5" s="21" t="s">
@@ -9372,67 +9384,67 @@
         <v>348</v>
       </c>
       <c r="I5" s="4">
-        <f>$C5*I$1</f>
+        <f t="shared" si="0"/>
         <v>163.5</v>
       </c>
       <c r="J5" s="4">
-        <f>$C5*J$1</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="K5" s="4">
-        <f>$C5*K$1</f>
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
       <c r="L5" s="4">
-        <f>$C5*L$1</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="M5" s="4">
-        <f>$C5*M$1</f>
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="N5" s="4">
-        <f>$C5*N$1</f>
+        <f t="shared" si="0"/>
         <v>292.5</v>
       </c>
       <c r="O5" s="4">
-        <f>$C5*O$1</f>
+        <f t="shared" si="0"/>
         <v>312</v>
       </c>
       <c r="P5" s="4">
-        <f>$C5*P$1</f>
+        <f t="shared" si="0"/>
         <v>340.5</v>
       </c>
       <c r="R5" s="4">
-        <f>$E5*R$1</f>
+        <f t="shared" si="1"/>
         <v>126.44</v>
       </c>
       <c r="S5" s="4">
-        <f>$E5*S$1</f>
+        <f t="shared" si="1"/>
         <v>139.19999999999999</v>
       </c>
       <c r="T5" s="4">
-        <f>$E5*T$1</f>
+        <f t="shared" si="1"/>
         <v>150.79999999999998</v>
       </c>
       <c r="U5" s="4">
-        <f>$E5*U$1</f>
+        <f t="shared" si="1"/>
         <v>162.39999999999998</v>
       </c>
       <c r="V5" s="4">
-        <f>$E5*V$1</f>
+        <f t="shared" si="1"/>
         <v>208.79999999999998</v>
       </c>
       <c r="W5" s="4">
-        <f>$E5*W$1</f>
+        <f t="shared" si="1"/>
         <v>226.2</v>
       </c>
       <c r="X5" s="4">
-        <f>$E5*X$1</f>
+        <f t="shared" si="1"/>
         <v>241.27999999999997</v>
       </c>
       <c r="Y5" s="4">
-        <f>$E5*Y$1</f>
+        <f t="shared" si="1"/>
         <v>263.32</v>
       </c>
     </row>
@@ -9444,14 +9456,14 @@
         <v>100</v>
       </c>
       <c r="C6" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
       <c r="D6" s="24">
         <v>249</v>
       </c>
       <c r="E6" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="F6" s="21" t="s">
@@ -9461,67 +9473,67 @@
         <v>348</v>
       </c>
       <c r="I6" s="4">
-        <f>$C6*I$1</f>
+        <f t="shared" si="0"/>
         <v>52.32</v>
       </c>
       <c r="J6" s="4">
-        <f>$C6*J$1</f>
+        <f t="shared" si="0"/>
         <v>57.599999999999994</v>
       </c>
       <c r="K6" s="4">
-        <f>$C6*K$1</f>
+        <f t="shared" si="0"/>
         <v>62.4</v>
       </c>
       <c r="L6" s="4">
-        <f>$C6*L$1</f>
+        <f t="shared" si="0"/>
         <v>67.2</v>
       </c>
       <c r="M6" s="4">
-        <f>$C6*M$1</f>
+        <f t="shared" si="0"/>
         <v>86.399999999999991</v>
       </c>
       <c r="N6" s="4">
-        <f>$C6*N$1</f>
+        <f t="shared" si="0"/>
         <v>93.6</v>
       </c>
       <c r="O6" s="4">
-        <f>$C6*O$1</f>
+        <f t="shared" si="0"/>
         <v>99.84</v>
       </c>
       <c r="P6" s="4">
-        <f>$C6*P$1</f>
+        <f t="shared" si="0"/>
         <v>108.96</v>
       </c>
       <c r="R6" s="4">
-        <f>$E6*R$1</f>
+        <f t="shared" si="1"/>
         <v>130.79999999999998</v>
       </c>
       <c r="S6" s="4">
-        <f>$E6*S$1</f>
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
       <c r="T6" s="4">
-        <f>$E6*T$1</f>
+        <f t="shared" si="1"/>
         <v>156</v>
       </c>
       <c r="U6" s="4">
-        <f>$E6*U$1</f>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="V6" s="4">
-        <f>$E6*V$1</f>
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
       <c r="W6" s="4">
-        <f>$E6*W$1</f>
+        <f t="shared" si="1"/>
         <v>234</v>
       </c>
       <c r="X6" s="4">
-        <f>$E6*X$1</f>
+        <f t="shared" si="1"/>
         <v>249.6</v>
       </c>
       <c r="Y6" s="4">
-        <f>$E6*Y$1</f>
+        <f t="shared" si="1"/>
         <v>272.39999999999998</v>
       </c>
     </row>
@@ -9533,14 +9545,14 @@
         <v>400</v>
       </c>
       <c r="C7" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
       <c r="D7" s="24">
         <v>227</v>
       </c>
       <c r="E7" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="F7" s="21" t="s">
@@ -9550,67 +9562,67 @@
         <v>348</v>
       </c>
       <c r="I7" s="4">
-        <f>$C7*I$1</f>
+        <f t="shared" si="0"/>
         <v>209.28</v>
       </c>
       <c r="J7" s="4">
-        <f>$C7*J$1</f>
+        <f t="shared" si="0"/>
         <v>230.39999999999998</v>
       </c>
       <c r="K7" s="4">
-        <f>$C7*K$1</f>
+        <f t="shared" si="0"/>
         <v>249.6</v>
       </c>
       <c r="L7" s="4">
-        <f>$C7*L$1</f>
+        <f t="shared" si="0"/>
         <v>268.8</v>
       </c>
       <c r="M7" s="4">
-        <f>$C7*M$1</f>
+        <f t="shared" si="0"/>
         <v>345.59999999999997</v>
       </c>
       <c r="N7" s="4">
-        <f>$C7*N$1</f>
+        <f t="shared" si="0"/>
         <v>374.4</v>
       </c>
       <c r="O7" s="4">
-        <f>$C7*O$1</f>
+        <f t="shared" si="0"/>
         <v>399.36</v>
       </c>
       <c r="P7" s="4">
-        <f>$C7*P$1</f>
+        <f t="shared" si="0"/>
         <v>435.84</v>
       </c>
       <c r="R7" s="4">
-        <f>$E7*R$1</f>
+        <f t="shared" si="1"/>
         <v>119.9</v>
       </c>
       <c r="S7" s="4">
-        <f>$E7*S$1</f>
+        <f t="shared" si="1"/>
         <v>132</v>
       </c>
       <c r="T7" s="4">
-        <f>$E7*T$1</f>
+        <f t="shared" si="1"/>
         <v>143</v>
       </c>
       <c r="U7" s="4">
-        <f>$E7*U$1</f>
+        <f t="shared" si="1"/>
         <v>154</v>
       </c>
       <c r="V7" s="4">
-        <f>$E7*V$1</f>
+        <f t="shared" si="1"/>
         <v>198.00000000000003</v>
       </c>
       <c r="W7" s="4">
-        <f>$E7*W$1</f>
+        <f t="shared" si="1"/>
         <v>214.50000000000003</v>
       </c>
       <c r="X7" s="4">
-        <f>$E7*X$1</f>
+        <f t="shared" si="1"/>
         <v>228.8</v>
       </c>
       <c r="Y7" s="4">
-        <f>$E7*Y$1</f>
+        <f t="shared" si="1"/>
         <v>249.70000000000002</v>
       </c>
     </row>
@@ -9622,14 +9634,14 @@
         <v>8</v>
       </c>
       <c r="C8" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="D8" s="24">
         <v>203</v>
       </c>
       <c r="E8" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.49</v>
       </c>
       <c r="F8" s="21" t="s">
@@ -9639,67 +9651,67 @@
         <v>351</v>
       </c>
       <c r="I8" s="4">
-        <f>$C8*I$1</f>
+        <f t="shared" si="0"/>
         <v>4.3600000000000003</v>
       </c>
       <c r="J8" s="4">
-        <f>$C8*J$1</f>
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="K8" s="4">
-        <f>$C8*K$1</f>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="L8" s="4">
-        <f>$C8*L$1</f>
+        <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
       <c r="M8" s="4">
-        <f>$C8*M$1</f>
+        <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
       <c r="N8" s="4">
-        <f>$C8*N$1</f>
+        <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
       <c r="O8" s="4">
-        <f>$C8*O$1</f>
+        <f t="shared" si="0"/>
         <v>8.32</v>
       </c>
       <c r="P8" s="4">
-        <f>$C8*P$1</f>
+        <f t="shared" si="0"/>
         <v>9.08</v>
       </c>
       <c r="R8" s="4">
-        <f>$E8*R$1</f>
+        <f t="shared" si="1"/>
         <v>106.82</v>
       </c>
       <c r="S8" s="4">
-        <f>$E8*S$1</f>
+        <f t="shared" si="1"/>
         <v>117.6</v>
       </c>
       <c r="T8" s="4">
-        <f>$E8*T$1</f>
+        <f t="shared" si="1"/>
         <v>127.39999999999999</v>
       </c>
       <c r="U8" s="4">
-        <f>$E8*U$1</f>
+        <f t="shared" si="1"/>
         <v>137.19999999999999</v>
       </c>
       <c r="V8" s="4">
-        <f>$E8*V$1</f>
+        <f t="shared" si="1"/>
         <v>176.4</v>
       </c>
       <c r="W8" s="4">
-        <f>$E8*W$1</f>
+        <f t="shared" si="1"/>
         <v>191.1</v>
       </c>
       <c r="X8" s="4">
-        <f>$E8*X$1</f>
+        <f t="shared" si="1"/>
         <v>203.84</v>
       </c>
       <c r="Y8" s="4">
-        <f>$E8*Y$1</f>
+        <f t="shared" si="1"/>
         <v>222.46</v>
       </c>
     </row>
@@ -9711,14 +9723,14 @@
         <v>400</v>
       </c>
       <c r="C9" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.96</v>
       </c>
       <c r="D9" s="24">
         <v>148</v>
       </c>
       <c r="E9" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -9728,67 +9740,67 @@
         <v>348</v>
       </c>
       <c r="I9" s="4">
-        <f>$C9*I$1</f>
+        <f t="shared" si="0"/>
         <v>209.28</v>
       </c>
       <c r="J9" s="4">
-        <f>$C9*J$1</f>
+        <f t="shared" si="0"/>
         <v>230.39999999999998</v>
       </c>
       <c r="K9" s="4">
-        <f>$C9*K$1</f>
+        <f t="shared" si="0"/>
         <v>249.6</v>
       </c>
       <c r="L9" s="4">
-        <f>$C9*L$1</f>
+        <f t="shared" si="0"/>
         <v>268.8</v>
       </c>
       <c r="M9" s="4">
-        <f>$C9*M$1</f>
+        <f t="shared" si="0"/>
         <v>345.59999999999997</v>
       </c>
       <c r="N9" s="4">
-        <f>$C9*N$1</f>
+        <f t="shared" si="0"/>
         <v>374.4</v>
       </c>
       <c r="O9" s="4">
-        <f>$C9*O$1</f>
+        <f t="shared" si="0"/>
         <v>399.36</v>
       </c>
       <c r="P9" s="4">
-        <f>$C9*P$1</f>
+        <f t="shared" si="0"/>
         <v>435.84</v>
       </c>
       <c r="R9" s="4">
-        <f>$E9*R$1</f>
+        <f t="shared" si="1"/>
         <v>78.48</v>
       </c>
       <c r="S9" s="4">
-        <f>$E9*S$1</f>
+        <f t="shared" si="1"/>
         <v>86.399999999999991</v>
       </c>
       <c r="T9" s="4">
-        <f>$E9*T$1</f>
+        <f t="shared" si="1"/>
         <v>93.6</v>
       </c>
       <c r="U9" s="4">
-        <f>$E9*U$1</f>
+        <f t="shared" si="1"/>
         <v>100.8</v>
       </c>
       <c r="V9" s="4">
-        <f>$E9*V$1</f>
+        <f t="shared" si="1"/>
         <v>129.6</v>
       </c>
       <c r="W9" s="4">
-        <f>$E9*W$1</f>
+        <f t="shared" si="1"/>
         <v>140.4</v>
       </c>
       <c r="X9" s="4">
-        <f>$E9*X$1</f>
+        <f t="shared" si="1"/>
         <v>149.76</v>
       </c>
       <c r="Y9" s="4">
-        <f>$E9*Y$1</f>
+        <f t="shared" si="1"/>
         <v>163.44</v>
       </c>
       <c r="AB9" s="9" t="s">
@@ -9813,14 +9825,14 @@
         <v>104</v>
       </c>
       <c r="C10" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="D10" s="24">
         <v>203</v>
       </c>
       <c r="E10" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.49</v>
       </c>
       <c r="F10" s="21" t="s">
@@ -9830,67 +9842,67 @@
         <v>348</v>
       </c>
       <c r="I10" s="4">
-        <f>$C10*I$1</f>
+        <f t="shared" si="0"/>
         <v>54.5</v>
       </c>
       <c r="J10" s="4">
-        <f>$C10*J$1</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="K10" s="4">
-        <f>$C10*K$1</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="L10" s="4">
-        <f>$C10*L$1</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="M10" s="4">
-        <f>$C10*M$1</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="N10" s="4">
-        <f>$C10*N$1</f>
+        <f t="shared" si="0"/>
         <v>97.5</v>
       </c>
       <c r="O10" s="4">
-        <f>$C10*O$1</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="P10" s="4">
-        <f>$C10*P$1</f>
+        <f t="shared" si="0"/>
         <v>113.5</v>
       </c>
       <c r="R10" s="4">
-        <f>$E10*R$1</f>
+        <f t="shared" si="1"/>
         <v>106.82</v>
       </c>
       <c r="S10" s="4">
-        <f>$E10*S$1</f>
+        <f t="shared" si="1"/>
         <v>117.6</v>
       </c>
       <c r="T10" s="4">
-        <f>$E10*T$1</f>
+        <f t="shared" si="1"/>
         <v>127.39999999999999</v>
       </c>
       <c r="U10" s="4">
-        <f>$E10*U$1</f>
+        <f t="shared" si="1"/>
         <v>137.19999999999999</v>
       </c>
       <c r="V10" s="4">
-        <f>$E10*V$1</f>
+        <f t="shared" si="1"/>
         <v>176.4</v>
       </c>
       <c r="W10" s="4">
-        <f>$E10*W$1</f>
+        <f t="shared" si="1"/>
         <v>191.1</v>
       </c>
       <c r="X10" s="4">
-        <f>$E10*X$1</f>
+        <f t="shared" si="1"/>
         <v>203.84</v>
       </c>
       <c r="Y10" s="4">
-        <f>$E10*Y$1</f>
+        <f t="shared" si="1"/>
         <v>222.46</v>
       </c>
       <c r="AB10" s="12" t="s">
@@ -9915,14 +9927,14 @@
         <v>73</v>
       </c>
       <c r="C11" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
       <c r="D11" s="24">
         <v>324</v>
       </c>
       <c r="E11" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="F11" s="21" t="s">
@@ -9932,67 +9944,67 @@
         <v>351</v>
       </c>
       <c r="I11" s="4">
-        <f>$C11*I$1</f>
+        <f t="shared" si="0"/>
         <v>39.24</v>
       </c>
       <c r="J11" s="4">
-        <f>$C11*J$1</f>
+        <f t="shared" si="0"/>
         <v>43.199999999999996</v>
       </c>
       <c r="K11" s="4">
-        <f>$C11*K$1</f>
+        <f t="shared" si="0"/>
         <v>46.8</v>
       </c>
       <c r="L11" s="4">
-        <f>$C11*L$1</f>
+        <f t="shared" si="0"/>
         <v>50.4</v>
       </c>
       <c r="M11" s="4">
-        <f>$C11*M$1</f>
+        <f t="shared" si="0"/>
         <v>64.8</v>
       </c>
       <c r="N11" s="4">
-        <f>$C11*N$1</f>
+        <f t="shared" si="0"/>
         <v>70.2</v>
       </c>
       <c r="O11" s="4">
-        <f>$C11*O$1</f>
+        <f t="shared" si="0"/>
         <v>74.88</v>
       </c>
       <c r="P11" s="4">
-        <f>$C11*P$1</f>
+        <f t="shared" si="0"/>
         <v>81.72</v>
       </c>
       <c r="R11" s="4">
-        <f>$E11*R$1</f>
+        <f t="shared" si="1"/>
         <v>170.04</v>
       </c>
       <c r="S11" s="4">
-        <f>$E11*S$1</f>
+        <f t="shared" si="1"/>
         <v>187.20000000000002</v>
       </c>
       <c r="T11" s="4">
-        <f>$E11*T$1</f>
+        <f t="shared" si="1"/>
         <v>202.8</v>
       </c>
       <c r="U11" s="4">
-        <f>$E11*U$1</f>
+        <f t="shared" si="1"/>
         <v>218.4</v>
       </c>
       <c r="V11" s="4">
-        <f>$E11*V$1</f>
+        <f t="shared" si="1"/>
         <v>280.8</v>
       </c>
       <c r="W11" s="4">
-        <f>$E11*W$1</f>
+        <f t="shared" si="1"/>
         <v>304.2</v>
       </c>
       <c r="X11" s="4">
-        <f>$E11*X$1</f>
+        <f t="shared" si="1"/>
         <v>324.48</v>
       </c>
       <c r="Y11" s="4">
-        <f>$E11*Y$1</f>
+        <f t="shared" si="1"/>
         <v>354.12</v>
       </c>
       <c r="AB11" s="15" t="s">
@@ -10017,14 +10029,14 @@
         <v>345</v>
       </c>
       <c r="C12" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.83</v>
       </c>
       <c r="D12" s="24">
         <v>324</v>
       </c>
       <c r="E12" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.78</v>
       </c>
       <c r="F12" s="21" t="s">
@@ -10034,67 +10046,67 @@
         <v>348</v>
       </c>
       <c r="I12" s="4">
-        <f>$C12*I$1</f>
+        <f t="shared" si="0"/>
         <v>180.94</v>
       </c>
       <c r="J12" s="4">
-        <f>$C12*J$1</f>
+        <f t="shared" si="0"/>
         <v>199.2</v>
       </c>
       <c r="K12" s="4">
-        <f>$C12*K$1</f>
+        <f t="shared" si="0"/>
         <v>215.79999999999998</v>
       </c>
       <c r="L12" s="4">
-        <f>$C12*L$1</f>
+        <f t="shared" si="0"/>
         <v>232.39999999999998</v>
       </c>
       <c r="M12" s="4">
-        <f>$C12*M$1</f>
+        <f t="shared" si="0"/>
         <v>298.8</v>
       </c>
       <c r="N12" s="4">
-        <f>$C12*N$1</f>
+        <f t="shared" si="0"/>
         <v>323.7</v>
       </c>
       <c r="O12" s="4">
-        <f>$C12*O$1</f>
+        <f t="shared" si="0"/>
         <v>345.28</v>
       </c>
       <c r="P12" s="4">
-        <f>$C12*P$1</f>
+        <f t="shared" si="0"/>
         <v>376.82</v>
       </c>
       <c r="R12" s="4">
-        <f>$E12*R$1</f>
+        <f t="shared" si="1"/>
         <v>170.04</v>
       </c>
       <c r="S12" s="4">
-        <f>$E12*S$1</f>
+        <f t="shared" si="1"/>
         <v>187.20000000000002</v>
       </c>
       <c r="T12" s="4">
-        <f>$E12*T$1</f>
+        <f t="shared" si="1"/>
         <v>202.8</v>
       </c>
       <c r="U12" s="4">
-        <f>$E12*U$1</f>
+        <f t="shared" si="1"/>
         <v>218.4</v>
       </c>
       <c r="V12" s="4">
-        <f>$E12*V$1</f>
+        <f t="shared" si="1"/>
         <v>280.8</v>
       </c>
       <c r="W12" s="4">
-        <f>$E12*W$1</f>
+        <f t="shared" si="1"/>
         <v>304.2</v>
       </c>
       <c r="X12" s="4">
-        <f>$E12*X$1</f>
+        <f t="shared" si="1"/>
         <v>324.48</v>
       </c>
       <c r="Y12" s="4">
-        <f>$E12*Y$1</f>
+        <f t="shared" si="1"/>
         <v>354.12</v>
       </c>
       <c r="AB12" s="12" t="s">
@@ -10119,14 +10131,14 @@
         <v>208</v>
       </c>
       <c r="C13" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="D13" s="24">
         <v>382</v>
       </c>
       <c r="E13" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.92</v>
       </c>
       <c r="F13" s="21" t="s">
@@ -10136,67 +10148,67 @@
         <v>345</v>
       </c>
       <c r="I13" s="4">
-        <f>$C13*I$1</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="J13" s="4">
-        <f>$C13*J$1</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="K13" s="4">
-        <f>$C13*K$1</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="L13" s="4">
-        <f>$C13*L$1</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="M13" s="4">
-        <f>$C13*M$1</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="N13" s="4">
-        <f>$C13*N$1</f>
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
       <c r="O13" s="4">
-        <f>$C13*O$1</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="P13" s="4">
-        <f>$C13*P$1</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="R13" s="4">
-        <f>$E13*R$1</f>
+        <f t="shared" si="1"/>
         <v>200.56</v>
       </c>
       <c r="S13" s="4">
-        <f>$E13*S$1</f>
+        <f t="shared" si="1"/>
         <v>220.8</v>
       </c>
       <c r="T13" s="4">
-        <f>$E13*T$1</f>
+        <f t="shared" si="1"/>
         <v>239.20000000000002</v>
       </c>
       <c r="U13" s="4">
-        <f>$E13*U$1</f>
+        <f t="shared" si="1"/>
         <v>257.60000000000002</v>
       </c>
       <c r="V13" s="4">
-        <f>$E13*V$1</f>
+        <f t="shared" si="1"/>
         <v>331.2</v>
       </c>
       <c r="W13" s="4">
-        <f>$E13*W$1</f>
+        <f t="shared" si="1"/>
         <v>358.8</v>
       </c>
       <c r="X13" s="4">
-        <f>$E13*X$1</f>
+        <f t="shared" si="1"/>
         <v>382.72</v>
       </c>
       <c r="Y13" s="4">
-        <f>$E13*Y$1</f>
+        <f t="shared" si="1"/>
         <v>417.68</v>
       </c>
       <c r="AB13" s="15" t="s">
@@ -10221,14 +10233,14 @@
         <v>386</v>
       </c>
       <c r="C14" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.93</v>
       </c>
       <c r="D14" s="24">
         <v>274</v>
       </c>
       <c r="E14" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.66</v>
       </c>
       <c r="F14" s="21" t="s">
@@ -10238,67 +10250,67 @@
         <v>351</v>
       </c>
       <c r="I14" s="4">
-        <f>$C14*I$1</f>
+        <f t="shared" si="0"/>
         <v>202.74</v>
       </c>
       <c r="J14" s="4">
-        <f>$C14*J$1</f>
+        <f t="shared" si="0"/>
         <v>223.20000000000002</v>
       </c>
       <c r="K14" s="4">
-        <f>$C14*K$1</f>
+        <f t="shared" si="0"/>
         <v>241.8</v>
       </c>
       <c r="L14" s="4">
-        <f>$C14*L$1</f>
+        <f t="shared" si="0"/>
         <v>260.40000000000003</v>
       </c>
       <c r="M14" s="4">
-        <f>$C14*M$1</f>
+        <f t="shared" si="0"/>
         <v>334.8</v>
       </c>
       <c r="N14" s="4">
-        <f>$C14*N$1</f>
+        <f t="shared" si="0"/>
         <v>362.70000000000005</v>
       </c>
       <c r="O14" s="4">
-        <f>$C14*O$1</f>
+        <f t="shared" si="0"/>
         <v>386.88</v>
       </c>
       <c r="P14" s="4">
-        <f>$C14*P$1</f>
+        <f t="shared" si="0"/>
         <v>422.22</v>
       </c>
       <c r="R14" s="4">
-        <f>$E14*R$1</f>
+        <f t="shared" si="1"/>
         <v>143.88</v>
       </c>
       <c r="S14" s="4">
-        <f>$E14*S$1</f>
+        <f t="shared" si="1"/>
         <v>158.4</v>
       </c>
       <c r="T14" s="4">
-        <f>$E14*T$1</f>
+        <f t="shared" si="1"/>
         <v>171.6</v>
       </c>
       <c r="U14" s="4">
-        <f>$E14*U$1</f>
+        <f t="shared" si="1"/>
         <v>184.8</v>
       </c>
       <c r="V14" s="4">
-        <f>$E14*V$1</f>
+        <f t="shared" si="1"/>
         <v>237.60000000000002</v>
       </c>
       <c r="W14" s="4">
-        <f>$E14*W$1</f>
+        <f t="shared" si="1"/>
         <v>257.40000000000003</v>
       </c>
       <c r="X14" s="4">
-        <f>$E14*X$1</f>
+        <f t="shared" si="1"/>
         <v>274.56</v>
       </c>
       <c r="Y14" s="4">
-        <f>$E14*Y$1</f>
+        <f t="shared" si="1"/>
         <v>299.64</v>
       </c>
       <c r="AB14" s="12" t="s">
@@ -10381,7 +10393,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="str">
-        <f t="shared" ref="A19:A31" si="1">""""&amp;A2&amp;"""=&gt;("&amp;C2&amp;" * largeurEcran),"</f>
+        <f t="shared" ref="A19:A31" si="3">""""&amp;A2&amp;"""=&gt;("&amp;C2&amp;" * largeurEcran),"</f>
         <v>"date"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B19" s="22"/>
@@ -10401,7 +10413,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"heure"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B20" s="22"/>
@@ -10421,7 +10433,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"notif"=&gt;(0.12 * largeurEcran),</v>
       </c>
       <c r="B21" s="22"/>
@@ -10441,7 +10453,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"BG"=&gt;(0.75 * largeurEcran),</v>
       </c>
       <c r="B22" s="22"/>
@@ -10461,7 +10473,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Delta"=&gt;(0.24 * largeurEcran),</v>
       </c>
       <c r="B23" s="22"/>
@@ -10481,7 +10493,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Elapsed"=&gt;(0.96 * largeurEcran),</v>
       </c>
       <c r="B24" s="22"/>
@@ -10501,7 +10513,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"ProvenanceBG"=&gt;(0.02 * largeurEcran),</v>
       </c>
       <c r="B25" s="22"/>
@@ -10521,7 +10533,7 @@
     </row>
     <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Secondes"=&gt;(0.96 * largeurEcran),</v>
       </c>
       <c r="B26" s="22"/>
@@ -10541,35 +10553,35 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"NextCall"=&gt;(0.25 * largeurEcran),</v>
       </c>
       <c r="B27" s="22"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Temperature"=&gt;(0.18 * largeurEcran),</v>
       </c>
       <c r="B28" s="22"/>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Wind"=&gt;(0.83 * largeurEcran),</v>
       </c>
       <c r="B29" s="22"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"Batterie"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B30" s="22"/>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>"labelMin"=&gt;(0.93 * largeurEcran),</v>
       </c>
       <c r="B31" s="22"/>
@@ -10599,84 +10611,84 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="str">
-        <f t="shared" ref="A36:A47" si="2">""""&amp;A3&amp;"""=&gt;"&amp;E3&amp;" * hauteurEcran,"</f>
+        <f t="shared" ref="A36:A47" si="4">""""&amp;A3&amp;"""=&gt;"&amp;E3&amp;" * hauteurEcran,"</f>
         <v>"heure"=&gt;0.31 * hauteurEcran,</v>
       </c>
       <c r="B36" s="22"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"notif"=&gt;0.39 * hauteurEcran,</v>
       </c>
       <c r="B37" s="22"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"BG"=&gt;0.58 * hauteurEcran,</v>
       </c>
       <c r="B38" s="22"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Delta"=&gt;0.6 * hauteurEcran,</v>
       </c>
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Elapsed"=&gt;0.55 * hauteurEcran,</v>
       </c>
       <c r="B40" s="22"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"ProvenanceBG"=&gt;0.49 * hauteurEcran,</v>
       </c>
       <c r="B41" s="22"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Secondes"=&gt;0.36 * hauteurEcran,</v>
       </c>
       <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"NextCall"=&gt;0.49 * hauteurEcran,</v>
       </c>
       <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Temperature"=&gt;0.78 * hauteurEcran,</v>
       </c>
       <c r="B44" s="22"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Wind"=&gt;0.78 * hauteurEcran,</v>
       </c>
       <c r="B45" s="22"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"Batterie"=&gt;0.92 * hauteurEcran,</v>
       </c>
       <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>"labelMin"=&gt;0.66 * hauteurEcran,</v>
       </c>
       <c r="B47" s="22"/>
@@ -10699,91 +10711,91 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="str">
-        <f t="shared" ref="A51:A63" si="3">""""&amp;A2&amp;"""=&gt;"&amp;F2&amp;","</f>
+        <f t="shared" ref="A51:A63" si="5">""""&amp;A2&amp;"""=&gt;"&amp;F2&amp;","</f>
         <v>"date"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B51" s="22"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"heure"=&gt;Gfx.FONT_NUMBER_HOT,</v>
       </c>
       <c r="B52" s="22"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"notif"=&gt;Gfx.FONT_MEDIUM,</v>
       </c>
       <c r="B53" s="22"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"BG"=&gt;Gfx.FONT_NUMBER_HOT,</v>
       </c>
       <c r="B54" s="22"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Delta"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B55" s="22"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Elapsed"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B56" s="22"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"ProvenanceBG"=&gt;Gfx.FONT_XTINY,</v>
       </c>
       <c r="B57" s="22"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Secondes"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B58" s="22"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"NextCall"=&gt;Gfx.FONT_XTINY,</v>
       </c>
       <c r="B59" s="22"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Temperature"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B60" s="22"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Wind"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B61" s="22"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"Batterie"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B62" s="22"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>"labelMin"=&gt;Gfx.FONT_XTINY,</v>
       </c>
       <c r="B63" s="22"/>
@@ -10813,84 +10825,84 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="str">
-        <f t="shared" ref="A68:A79" si="4">""""&amp;A3&amp;"""=&gt;"&amp;G3&amp;","</f>
+        <f t="shared" ref="A68:A79" si="6">""""&amp;A3&amp;"""=&gt;"&amp;G3&amp;","</f>
         <v>"heure"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B68" s="22"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"notif"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B69" s="22"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"BG"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B70" s="22"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Delta"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B71" s="22"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Elapsed"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B72" s="22"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"ProvenanceBG"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B73" s="22"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Secondes"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B74" s="22"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"NextCall"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B75" s="22"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Temperature"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B76" s="22"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Wind"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B77" s="22"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Batterie"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B78" s="22"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"labelMin"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B79" s="22"/>
@@ -12220,8 +12232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12267,22 +12279,22 @@
         <v>1744806142000</v>
       </c>
       <c r="B2">
-        <f>A2/1000/60/60/24</f>
+        <f t="shared" ref="B2:B12" si="0">A2/1000/60/60/24</f>
         <v>20194.515532407408</v>
       </c>
       <c r="C2" s="6">
-        <f>TRUNC((B2)+DATE(1970,1,1),0)</f>
+        <f t="shared" ref="C2:C12" si="1">TRUNC((B2)+DATE(1970,1,1),0)</f>
         <v>45763</v>
       </c>
       <c r="D2" s="7">
-        <f>B2-TRUNC(B2,0)</f>
+        <f t="shared" ref="D2:D12" si="2">B2-TRUNC(B2,0)</f>
         <v>0.51553240740759065</v>
       </c>
       <c r="E2" s="7">
-        <f>D2+1/12</f>
+        <f t="shared" ref="E2:E12" si="3">D2+1/12</f>
         <v>0.59886574074092402</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="4">
         <v>1744698759</v>
       </c>
       <c r="I2">
@@ -12307,22 +12319,22 @@
         <v>1744806293000</v>
       </c>
       <c r="B3">
-        <f>A3/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.51728009259</v>
       </c>
       <c r="C3" s="6">
-        <f>TRUNC((B3)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D3" s="7">
-        <f>B3-TRUNC(B3,0)</f>
+        <f t="shared" si="2"/>
         <v>0.51728009259022656</v>
       </c>
       <c r="E3" s="7">
-        <f>D3+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.60061342592355993</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="4">
         <v>1744804492</v>
       </c>
       <c r="I3">
@@ -12347,22 +12359,22 @@
         <v>1744806293000</v>
       </c>
       <c r="B4">
-        <f>A4/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.51728009259</v>
       </c>
       <c r="C4" s="6">
-        <f>TRUNC((B4)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D4" s="7">
-        <f>B4-TRUNC(B4,0)</f>
+        <f t="shared" si="2"/>
         <v>0.51728009259022656</v>
       </c>
       <c r="E4" s="7">
-        <f>D4+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.60061342592355993</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>1744814539</v>
       </c>
       <c r="I4">
@@ -12387,22 +12399,22 @@
         <v>1744806442000</v>
       </c>
       <c r="B5">
-        <f>A5/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.51900462963</v>
       </c>
       <c r="C5" s="6">
-        <f>TRUNC((B5)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D5" s="7">
-        <f>B5-TRUNC(B5,0)</f>
+        <f t="shared" si="2"/>
         <v>0.5190046296302171</v>
       </c>
       <c r="E5" s="7">
-        <f>D5+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.60233796296355047</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="4">
         <v>1744817093</v>
       </c>
       <c r="I5">
@@ -12427,19 +12439,19 @@
         <v>1744806442000</v>
       </c>
       <c r="B6">
-        <f>A6/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.51900462963</v>
       </c>
       <c r="C6" s="6">
-        <f>TRUNC((B6)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D6" s="7">
-        <f>B6-TRUNC(B6,0)</f>
+        <f t="shared" si="2"/>
         <v>0.5190046296302171</v>
       </c>
       <c r="E6" s="7">
-        <f>D6+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.60233796296355047</v>
       </c>
     </row>
@@ -12448,20 +12460,26 @@
         <v>1744806592000</v>
       </c>
       <c r="B7">
-        <f>A7/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.52074074074</v>
       </c>
       <c r="C7" s="6">
-        <f>TRUNC((B7)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D7" s="7">
-        <f>B7-TRUNC(B7,0)</f>
+        <f t="shared" si="2"/>
         <v>0.52074074073971133</v>
       </c>
       <c r="E7" s="7">
-        <f>D7+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.6040740740730447</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1746796363180</v>
+      </c>
+      <c r="I7" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -12469,20 +12487,26 @@
         <v>1744806592000</v>
       </c>
       <c r="B8">
-        <f>A8/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.52074074074</v>
       </c>
       <c r="C8" s="6">
-        <f>TRUNC((B8)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D8" s="7">
-        <f>B8-TRUNC(B8,0)</f>
+        <f t="shared" si="2"/>
         <v>0.52074074073971133</v>
       </c>
       <c r="E8" s="7">
-        <f>D8+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.6040740740730447</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1744817093</v>
+      </c>
+      <c r="I8" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -12490,19 +12514,19 @@
         <v>1744806742000</v>
       </c>
       <c r="B9">
-        <f>A9/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.522476851853</v>
       </c>
       <c r="C9" s="6">
-        <f>TRUNC((B9)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D9" s="7">
-        <f>B9-TRUNC(B9,0)</f>
+        <f t="shared" si="2"/>
         <v>0.52247685185284354</v>
       </c>
       <c r="E9" s="7">
-        <f>D9+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.60581018518617691</v>
       </c>
     </row>
@@ -12511,27 +12535,69 @@
         <v>1744813193000</v>
       </c>
       <c r="B10">
-        <f>A10/1000/60/60/24</f>
+        <f t="shared" si="0"/>
         <v>20194.597141203703</v>
       </c>
       <c r="C10" s="6">
-        <f>TRUNC((B10)+DATE(1970,1,1),0)</f>
+        <f t="shared" si="1"/>
         <v>45763</v>
       </c>
       <c r="D10" s="7">
-        <f>B10-TRUNC(B10,0)</f>
+        <f t="shared" si="2"/>
         <v>0.59714120370335877</v>
       </c>
       <c r="E10" s="7">
-        <f>D10+1/12</f>
+        <f t="shared" si="3"/>
         <v>0.68047453703669214</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1746687349622</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>20216.288768773149</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>45785</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="2"/>
+        <v>0.28876877314905869</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="3"/>
+        <v>0.372102106482392</v>
+      </c>
+      <c r="F11" t="s">
+        <v>571</v>
+      </c>
+    </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="4">
+        <v>1746686742872</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>20216.281746203702</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="1"/>
+        <v>45785</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="2"/>
+        <v>0.28174620370191406</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="3"/>
+        <v>0.36507953703524737</v>
+      </c>
+      <c r="F12" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>

</xml_diff>

<commit_message>
supprime logo bluetooth pour mémoire
</commit_message>
<xml_diff>
--- a/Modèles.xlsx
+++ b/Modèles.xlsx
@@ -13,16 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="modèles" sheetId="1" r:id="rId1"/>
-    <sheet name="écran" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil5" sheetId="5" r:id="rId3"/>
-    <sheet name="manifest" sheetId="3" r:id="rId4"/>
-    <sheet name="calculs" sheetId="4" r:id="rId5"/>
+    <sheet name="BT" sheetId="6" r:id="rId2"/>
+    <sheet name="écran" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil5" sheetId="5" r:id="rId4"/>
+    <sheet name="manifest" sheetId="3" r:id="rId5"/>
+    <sheet name="calculs" sheetId="4" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">manifest!$A$1:$A$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">manifest!$A$1:$A$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">modèles!$A$1:$N$139</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="583">
   <si>
     <t>deviceId</t>
   </si>
@@ -1757,6 +1758,33 @@
   </si>
   <si>
     <t>secondes</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>ligne</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2*</t>
   </si>
 </sst>
 </file>
@@ -2030,6 +2058,387 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6145" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>144859</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886576" y="381000"/>
+          <a:ext cx="3448050" cy="3383359"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 1" descr="File:Bluetooth.svg - Wikipedia"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2286000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2661,12 +3070,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O139"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117:XFD117"/>
+      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2724,7 +3134,7 @@
       </c>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2762,12 +3172,11 @@
         <f>IFERROR(VLOOKUP(A2,manifest!A:A,1,0),"")</f>
         <v>approachs50</v>
       </c>
-      <c r="N2" t="str">
-        <f>"&lt;iq:product id="""&amp;A2&amp;"""/&gt;"</f>
-        <v>&lt;iq:product id="approachs50"/&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2813,7 +3222,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2859,7 +3268,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2900,12 +3309,11 @@
         <f>IFERROR(VLOOKUP(A5,manifest!A:A,1,0),"")</f>
         <v>approachs7042mm</v>
       </c>
-      <c r="N5" t="str">
-        <f t="shared" ref="N5:N6" si="0">"&lt;iq:product id="""&amp;A5&amp;"""/&gt;"</f>
-        <v>&lt;iq:product id="approachs7042mm"/&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2946,12 +3354,11 @@
         <f>IFERROR(VLOOKUP(A6,manifest!A:A,1,0),"")</f>
         <v>approachs7047mm</v>
       </c>
-      <c r="N6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;iq:product id="approachs7047mm"/&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2997,7 +3404,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -3038,12 +3445,11 @@
         <f>IFERROR(VLOOKUP(A8,manifest!A:A,1,0),"")</f>
         <v>d2air</v>
       </c>
-      <c r="N8" t="str">
-        <f t="shared" ref="N8:N9" si="1">"&lt;iq:product id="""&amp;A8&amp;"""/&gt;"</f>
-        <v>&lt;iq:product id="d2air"/&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3084,12 +3490,11 @@
         <f>IFERROR(VLOOKUP(A9,manifest!A:A,1,0),"")</f>
         <v>d2airx10</v>
       </c>
-      <c r="N9" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;iq:product id="d2airx10"/&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3135,7 +3540,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3181,7 +3586,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3269,8 +3674,8 @@
         <v>d2delta</v>
       </c>
       <c r="N13" t="str">
-        <f>A13&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>d2delta.excludeAnnotations="noMenus"</v>
+        <f>A13&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>d2delta.excludeAnnotations="onlyWithSettingOnWatchface"</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3315,8 +3720,8 @@
         <v>d2deltapx</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" ref="N14:N15" si="2">A14&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>d2deltapx.excludeAnnotations="noMenus"</v>
+        <f t="shared" ref="N14:N15" si="0">A14&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>d2deltapx.excludeAnnotations="onlyWithSettingOnWatchface"</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3361,11 +3766,11 @@
         <v>d2deltas</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="2"/>
-        <v>d2deltas.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>d2deltas.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -3410,7 +3815,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -3456,7 +3861,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3501,7 +3906,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -3547,7 +3952,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -3592,7 +3997,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -3637,7 +4042,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -3682,7 +4087,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -3727,7 +4132,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -3772,7 +4177,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -3817,7 +4222,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -3863,7 +4268,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -3908,7 +4313,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -3953,7 +4358,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -3998,7 +4403,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -4043,7 +4448,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -4089,7 +4494,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -4177,11 +4582,11 @@
         <v>fenix5</v>
       </c>
       <c r="N33" t="str">
-        <f>A33&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fenix5.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A33&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fenix5.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -4268,11 +4673,11 @@
         <v>fenix5s</v>
       </c>
       <c r="N35" t="str">
-        <f>A35&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fenix5s.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A35&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fenix5s.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -4359,11 +4764,11 @@
         <v>fenix5x</v>
       </c>
       <c r="N37" t="str">
-        <f>A37&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fenix5x.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A37&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fenix5x.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -4408,7 +4813,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -4453,7 +4858,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -4498,7 +4903,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -4543,7 +4948,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -4588,7 +4993,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -4633,7 +5038,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -4678,7 +5083,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -4723,7 +5128,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -4768,7 +5173,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -4813,7 +5218,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -4858,7 +5263,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -4903,7 +5308,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -4948,7 +5353,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>136</v>
       </c>
@@ -4993,7 +5398,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -5038,7 +5443,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -5083,7 +5488,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -5128,7 +5533,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>144</v>
       </c>
@@ -5215,11 +5620,11 @@
         <v>fenixchronos</v>
       </c>
       <c r="N56" t="str">
-        <f>A56&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fenixchronos.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A56&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fenixchronos.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -5264,7 +5669,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>150</v>
       </c>
@@ -5309,7 +5714,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>152</v>
       </c>
@@ -5354,7 +5759,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>154</v>
       </c>
@@ -5400,7 +5805,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>157</v>
       </c>
@@ -5446,7 +5851,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>159</v>
       </c>
@@ -5491,7 +5896,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>162</v>
       </c>
@@ -5536,7 +5941,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -5581,7 +5986,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>166</v>
       </c>
@@ -5626,7 +6031,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>168</v>
       </c>
@@ -5671,7 +6076,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>170</v>
       </c>
@@ -5716,7 +6121,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>172</v>
       </c>
@@ -5761,7 +6166,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>174</v>
       </c>
@@ -5806,7 +6211,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -5852,7 +6257,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>181</v>
       </c>
@@ -5898,7 +6303,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>183</v>
       </c>
@@ -5943,7 +6348,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>185</v>
       </c>
@@ -5988,7 +6393,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>187</v>
       </c>
@@ -6076,11 +6481,11 @@
         <v>fr645</v>
       </c>
       <c r="N75" t="str">
-        <f>A75&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fr645.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A75&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fr645.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>191</v>
       </c>
@@ -6125,7 +6530,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -6171,7 +6576,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -6216,7 +6621,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>198</v>
       </c>
@@ -6304,11 +6709,11 @@
         <v>fr935</v>
       </c>
       <c r="N80" t="str">
-        <f>A80&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>fr935.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A80&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>fr935.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>202</v>
       </c>
@@ -6353,7 +6758,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>204</v>
       </c>
@@ -6398,7 +6803,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -6443,7 +6848,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>209</v>
       </c>
@@ -6488,7 +6893,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>211</v>
       </c>
@@ -6533,7 +6938,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>213</v>
       </c>
@@ -6579,7 +6984,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -6625,7 +7030,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>217</v>
       </c>
@@ -6671,7 +7076,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>220</v>
       </c>
@@ -6717,7 +7122,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>222</v>
       </c>
@@ -6762,7 +7167,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>224</v>
       </c>
@@ -6807,7 +7212,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>226</v>
       </c>
@@ -6853,7 +7258,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>460</v>
       </c>
@@ -6899,7 +7304,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>228</v>
       </c>
@@ -6945,7 +7350,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>230</v>
       </c>
@@ -6991,7 +7396,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>233</v>
       </c>
@@ -7033,11 +7438,11 @@
         <v/>
       </c>
       <c r="N96" t="str">
-        <f t="shared" ref="N96" si="3">"&lt;iq:product id="""&amp;A96&amp;"""/&gt;"</f>
+        <f t="shared" ref="N96" si="1">"&lt;iq:product id="""&amp;A96&amp;"""/&gt;"</f>
         <v>&lt;iq:product id="instincte45mm"/&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>235</v>
       </c>
@@ -7082,7 +7487,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>238</v>
       </c>
@@ -7127,7 +7532,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>241</v>
       </c>
@@ -7172,7 +7577,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>243</v>
       </c>
@@ -7217,7 +7622,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>245</v>
       </c>
@@ -7259,11 +7664,11 @@
         <v/>
       </c>
       <c r="N101" t="str">
-        <f t="shared" ref="N101:N112" si="4">"&lt;iq:product id="""&amp;A101&amp;"""/&gt;"</f>
+        <f t="shared" ref="N101:N112" si="2">"&lt;iq:product id="""&amp;A101&amp;"""/&gt;"</f>
         <v>&lt;iq:product id="lily2"/&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>249</v>
       </c>
@@ -7308,7 +7713,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>251</v>
       </c>
@@ -7353,7 +7758,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>253</v>
       </c>
@@ -7398,7 +7803,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>255</v>
       </c>
@@ -7443,7 +7848,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>257</v>
       </c>
@@ -7488,7 +7893,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>259</v>
       </c>
@@ -7533,7 +7938,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>261</v>
       </c>
@@ -7578,7 +7983,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>263</v>
       </c>
@@ -7623,7 +8028,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>265</v>
       </c>
@@ -7668,7 +8073,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>267</v>
       </c>
@@ -7713,7 +8118,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>477</v>
       </c>
@@ -7755,11 +8160,11 @@
         <v/>
       </c>
       <c r="N112" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>&lt;iq:product id="system8preview"/&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>269</v>
       </c>
@@ -7804,7 +8209,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>271</v>
       </c>
@@ -7849,7 +8254,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>273</v>
       </c>
@@ -7894,7 +8299,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>275</v>
       </c>
@@ -7939,7 +8344,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>277</v>
       </c>
@@ -7984,7 +8389,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>279</v>
       </c>
@@ -8029,7 +8434,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>281</v>
       </c>
@@ -8074,7 +8479,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>283</v>
       </c>
@@ -8119,7 +8524,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>285</v>
       </c>
@@ -8164,7 +8569,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>288</v>
       </c>
@@ -8210,7 +8615,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>290</v>
       </c>
@@ -8256,7 +8661,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>293</v>
       </c>
@@ -8302,7 +8707,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>295</v>
       </c>
@@ -8348,7 +8753,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>297</v>
       </c>
@@ -8394,7 +8799,7 @@
         <v>&lt;iq:product id="venux1"/&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>300</v>
       </c>
@@ -8482,11 +8887,11 @@
         <v>vivoactive3</v>
       </c>
       <c r="N128" t="str">
-        <f>A128&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>vivoactive3.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+        <f>A128&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>vivoactive3.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>305</v>
       </c>
@@ -8528,7 +8933,7 @@
         <v/>
       </c>
       <c r="N129" t="str">
-        <f t="shared" ref="N129" si="5">"&lt;iq:product id="""&amp;A129&amp;"""/&gt;"</f>
+        <f t="shared" ref="N129" si="3">"&lt;iq:product id="""&amp;A129&amp;"""/&gt;"</f>
         <v>&lt;iq:product id="vivoactive3d"/&gt;</v>
       </c>
     </row>
@@ -8573,8 +8978,9 @@
         <f>IFERROR(VLOOKUP(A130,manifest!A:A,1,0),"")</f>
         <v>vivoactive3m</v>
       </c>
-      <c r="N130" t="s">
-        <v>511</v>
+      <c r="N130" t="str">
+        <f t="shared" ref="N130:N131" si="4">A130&amp;".excludeAnnotations=""onlyWithSettingOnWatchface"""</f>
+        <v>vivoactive3m.excludeAnnotations="onlyWithSettingOnWatchface"</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
@@ -8619,11 +9025,11 @@
         <v>vivoactive3mlte</v>
       </c>
       <c r="N131" t="str">
-        <f>A131&amp;".excludeAnnotations=""noMenus"""</f>
-        <v>vivoactive3mlte.excludeAnnotations="noMenus"</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>vivoactive3mlte.excludeAnnotations="onlyWithSettingOnWatchface"</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>311</v>
       </c>
@@ -8668,7 +9074,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>313</v>
       </c>
@@ -8713,7 +9119,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>315</v>
       </c>
@@ -8758,7 +9164,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>317</v>
       </c>
@@ -8803,7 +9209,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>319</v>
       </c>
@@ -8845,11 +9251,11 @@
         <v/>
       </c>
       <c r="N136" t="str">
-        <f t="shared" ref="N136:N137" si="6">"&lt;iq:product id="""&amp;A136&amp;"""/&gt;"</f>
+        <f t="shared" ref="N136:N137" si="5">"&lt;iq:product id="""&amp;A136&amp;"""/&gt;"</f>
         <v>&lt;iq:product id="vivoactive_hr"/&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>322</v>
       </c>
@@ -8891,11 +9297,11 @@
         <v/>
       </c>
       <c r="N137" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>&lt;iq:product id="vivolife"/&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>326</v>
       </c>
@@ -8937,7 +9343,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>329</v>
       </c>
@@ -8979,8 +9385,66 @@
         <v/>
       </c>
     </row>
+    <row r="145" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="146" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>142</v>
+      </c>
+      <c r="E146">
+        <f>D146/D145</f>
+        <v>0.34134615384615385</v>
+      </c>
+    </row>
+    <row r="147" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E147">
+        <f>1-E146</f>
+        <v>0.65865384615384615</v>
+      </c>
+    </row>
+    <row r="148" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H148">
+        <f>0.5-0.16</f>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="J148">
+        <f>0.375-0.625</f>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="149" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H149">
+        <f>0.16*2</f>
+        <v>0.32</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N139"/>
+  <autoFilter ref="A1:N139">
+    <filterColumn colId="12">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="13">
+      <filters>
+        <filter val="d2delta.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="d2deltapx.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="d2deltas.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fenix5.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fenix5s.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fenix5x.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fenixchronos.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fr645.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="fr935.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="vivoactive3.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="vivoactive3m.excludeAnnotations=&quot;noMenus&quot;"/>
+        <filter val="vivoactive3mlte.excludeAnnotations=&quot;noMenus&quot;"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8988,9 +9452,389 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1" t="s">
+        <v>575</v>
+      </c>
+      <c r="E1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"centrex+"&amp;B2&amp;"*tailleLogo"</f>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"centrey+"&amp;C2&amp;"*tailleLogo"</f>
+        <v>centrey+0*tailleLogo</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-0.5</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E8" si="0">"centrex+"&amp;B3&amp;"*tailleLogo"</f>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F8" si="1">"centrey+"&amp;C3&amp;"*tailleLogo"</f>
+        <v>centrey+-0.5*tailleLogo</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>centrey+0.5*tailleLogo</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-0.25</v>
+      </c>
+      <c r="C5">
+        <v>-0.25</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>centrex+-0.25*tailleLogo</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>centrey+-0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6">
+        <v>-0.25</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>centrey+-0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>-0.25</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>centrex+-0.25*tailleLogo</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>centrey+0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.25</v>
+      </c>
+      <c r="C8">
+        <v>0.25</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>centrey+0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B11" t="s">
+        <v>578</v>
+      </c>
+      <c r="C11" t="s">
+        <v>578</v>
+      </c>
+      <c r="E11" t="s">
+        <v>579</v>
+      </c>
+      <c r="F11" t="s">
+        <v>580</v>
+      </c>
+      <c r="G11" t="s">
+        <v>581</v>
+      </c>
+      <c r="H11" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f>VLOOKUP(B12,$A$2:$F$8,5,0)</f>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F12" t="str">
+        <f>VLOOKUP(B12,$A$2:$F$8,6,0)</f>
+        <v>centrey+-0.5*tailleLogo</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(C12,$A$2:$F$8,5,0)</f>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="H12" t="str">
+        <f>VLOOKUP(C12,$A$2:$F$8,6,0)</f>
+        <v>centrey+0.5*tailleLogo</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" ref="E13:E16" si="2">VLOOKUP(B13,$A$2:$F$8,5,0)</f>
+        <v>centrex+-0.25*tailleLogo</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F16" si="3">VLOOKUP(B13,$A$2:$F$8,6,0)</f>
+        <v>centrey+-0.25*tailleLogo</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G16" si="4">VLOOKUP(C13,$A$2:$F$8,5,0)</f>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ref="H13:H16" si="5">VLOOKUP(C13,$A$2:$F$8,6,0)</f>
+        <v>centrey+0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>centrex+-0.25*tailleLogo</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>centrey+0.25*tailleLogo</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="4"/>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="5"/>
+        <v>centrey+-0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>centrey+-0.5*tailleLogo</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="4"/>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="5"/>
+        <v>centrey+-0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>centrex+0*tailleLogo</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>centrey+0.5*tailleLogo</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="4"/>
+        <v>centrex+0.25*tailleLogo</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="5"/>
+        <v>centrey+0.25*tailleLogo</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="str">
+        <f>"dc.drawLine("&amp;E12&amp;","&amp;F12&amp;","&amp;G12&amp;","&amp;H12&amp;");"</f>
+        <v>dc.drawLine(centrex+0*tailleLogo,centrey+-0.5*tailleLogo,centrex+0*tailleLogo,centrey+0.5*tailleLogo);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" ref="E22:E25" si="6">"dc.drawLine("&amp;E13&amp;","&amp;F13&amp;","&amp;G13&amp;","&amp;H13&amp;");"</f>
+        <v>dc.drawLine(centrex+-0.25*tailleLogo,centrey+-0.25*tailleLogo,centrex+0.25*tailleLogo,centrey+0.25*tailleLogo);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="6"/>
+        <v>dc.drawLine(centrex+-0.25*tailleLogo,centrey+0.25*tailleLogo,centrex+0.25*tailleLogo,centrey+-0.25*tailleLogo);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="6"/>
+        <v>dc.drawLine(centrex+0*tailleLogo,centrey+-0.5*tailleLogo,centrex+0.25*tailleLogo,centrey+-0.25*tailleLogo);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="6"/>
+        <v>dc.drawLine(centrex+0*tailleLogo,centrey+0.5*tailleLogo,centrex+0.25*tailleLogo,centrey+0.25*tailleLogo);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
@@ -10288,7 +11132,7 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="str">
-        <f>""""&amp;A2&amp;"""=&gt;("&amp;C2&amp;" * largeurEcran),"</f>
+        <f t="shared" ref="A18:A25" si="3">""""&amp;A2&amp;"""=&gt;("&amp;C2&amp;" * largeurEcran),"</f>
         <v>"date"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B18" s="22"/>
@@ -10308,7 +11152,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="str">
-        <f>""""&amp;A3&amp;"""=&gt;("&amp;C3&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"heure"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B19" s="22"/>
@@ -10328,7 +11172,7 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="str">
-        <f>""""&amp;A4&amp;"""=&gt;("&amp;C4&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"notif"=&gt;(0.12 * largeurEcran),</v>
       </c>
       <c r="B20" s="22"/>
@@ -10348,7 +11192,7 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="str">
-        <f>""""&amp;A5&amp;"""=&gt;("&amp;C5&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"BG"=&gt;(0.75 * largeurEcran),</v>
       </c>
       <c r="B21" s="22"/>
@@ -10368,7 +11212,7 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="str">
-        <f>""""&amp;A6&amp;"""=&gt;("&amp;C6&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"Delta"=&gt;(0.24 * largeurEcran),</v>
       </c>
       <c r="B22" s="22"/>
@@ -10388,7 +11232,7 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
-        <f>""""&amp;A7&amp;"""=&gt;("&amp;C7&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"Elapsed"=&gt;(0.96 * largeurEcran),</v>
       </c>
       <c r="B23" s="22"/>
@@ -10408,7 +11252,7 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
-        <f>""""&amp;A8&amp;"""=&gt;("&amp;C8&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"ProvenanceBG"=&gt;(0.02 * largeurEcran),</v>
       </c>
       <c r="B24" s="22"/>
@@ -10428,7 +11272,7 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
-        <f>""""&amp;A9&amp;"""=&gt;("&amp;C9&amp;" * largeurEcran),"</f>
+        <f t="shared" si="3"/>
         <v>"Secondes"=&gt;(0.96 * largeurEcran),</v>
       </c>
       <c r="B25" s="22"/>
@@ -10448,7 +11292,7 @@
     </row>
     <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="str">
-        <f t="shared" ref="A26:A29" si="3">""""&amp;A10&amp;"""=&gt;("&amp;C10&amp;" * largeurEcran),"</f>
+        <f t="shared" ref="A26:A29" si="4">""""&amp;A10&amp;"""=&gt;("&amp;C10&amp;" * largeurEcran),"</f>
         <v>"Temperature"=&gt;(0.18 * largeurEcran),</v>
       </c>
       <c r="B26" s="22"/>
@@ -10468,21 +11312,21 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Wind"=&gt;(0.83 * largeurEcran),</v>
       </c>
       <c r="B27" s="22"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"Batterie"=&gt;(0.5 * largeurEcran),</v>
       </c>
       <c r="B28" s="22"/>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>"labelMin"=&gt;(0.93 * largeurEcran),</v>
       </c>
       <c r="B29" s="22"/>
@@ -10512,77 +11356,77 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="str">
-        <f>""""&amp;A3&amp;"""=&gt;"&amp;E3&amp;" * hauteurEcran,"</f>
+        <f t="shared" ref="A34:A40" si="5">""""&amp;A3&amp;"""=&gt;"&amp;E3&amp;" * hauteurEcran,"</f>
         <v>"heure"=&gt;0.31 * hauteurEcran,</v>
       </c>
       <c r="B34" s="22"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="str">
-        <f>""""&amp;A4&amp;"""=&gt;"&amp;E4&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"notif"=&gt;0.39 * hauteurEcran,</v>
       </c>
       <c r="B35" s="22"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="str">
-        <f>""""&amp;A5&amp;"""=&gt;"&amp;E5&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"BG"=&gt;0.58 * hauteurEcran,</v>
       </c>
       <c r="B36" s="22"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="str">
-        <f>""""&amp;A6&amp;"""=&gt;"&amp;E6&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"Delta"=&gt;0.6 * hauteurEcran,</v>
       </c>
       <c r="B37" s="22"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="str">
-        <f>""""&amp;A7&amp;"""=&gt;"&amp;E7&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"Elapsed"=&gt;0.55 * hauteurEcran,</v>
       </c>
       <c r="B38" s="22"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="str">
-        <f>""""&amp;A8&amp;"""=&gt;"&amp;E8&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"ProvenanceBG"=&gt;0.49 * hauteurEcran,</v>
       </c>
       <c r="B39" s="22"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="str">
-        <f>""""&amp;A9&amp;"""=&gt;"&amp;E9&amp;" * hauteurEcran,"</f>
+        <f t="shared" si="5"/>
         <v>"Secondes"=&gt;0.36 * hauteurEcran,</v>
       </c>
       <c r="B40" s="22"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="str">
-        <f t="shared" ref="A41:A44" si="4">""""&amp;A10&amp;"""=&gt;"&amp;E10&amp;" * hauteurEcran,"</f>
+        <f t="shared" ref="A41:A44" si="6">""""&amp;A10&amp;"""=&gt;"&amp;E10&amp;" * hauteurEcran,"</f>
         <v>"Temperature"=&gt;0.78 * hauteurEcran,</v>
       </c>
       <c r="B41" s="22"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Wind"=&gt;0.78 * hauteurEcran,</v>
       </c>
       <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"Batterie"=&gt;0.92 * hauteurEcran,</v>
       </c>
       <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>"labelMin"=&gt;0.66 * hauteurEcran,</v>
       </c>
       <c r="B44" s="22"/>
@@ -10605,84 +11449,84 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="str">
-        <f>""""&amp;A2&amp;"""=&gt;"&amp;F2&amp;","</f>
+        <f t="shared" ref="A48:A55" si="7">""""&amp;A2&amp;"""=&gt;"&amp;F2&amp;","</f>
         <v>"date"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B48" s="22"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="str">
-        <f>""""&amp;A3&amp;"""=&gt;"&amp;F3&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"heure"=&gt;Gfx.FONT_NUMBER_HOT,</v>
       </c>
       <c r="B49" s="23"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="str">
-        <f>""""&amp;A4&amp;"""=&gt;"&amp;F4&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"notif"=&gt;Gfx.FONT_MEDIUM,</v>
       </c>
       <c r="B50" s="22"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="str">
-        <f>""""&amp;A5&amp;"""=&gt;"&amp;F5&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"BG"=&gt;Gfx.FONT_NUMBER_HOT,</v>
       </c>
       <c r="B51" s="22"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="str">
-        <f>""""&amp;A6&amp;"""=&gt;"&amp;F6&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"Delta"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B52" s="22"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="str">
-        <f>""""&amp;A7&amp;"""=&gt;"&amp;F7&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"Elapsed"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B53" s="22"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="str">
-        <f>""""&amp;A8&amp;"""=&gt;"&amp;F8&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"ProvenanceBG"=&gt;Gfx.FONT_XTINY,</v>
       </c>
       <c r="B54" s="22"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="str">
-        <f>""""&amp;A9&amp;"""=&gt;"&amp;F9&amp;","</f>
+        <f t="shared" si="7"/>
         <v>"Secondes"=&gt;Gfx.FONT_NUMBER_MILD,</v>
       </c>
       <c r="B55" s="22"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="str">
-        <f t="shared" ref="A56:A59" si="5">""""&amp;A10&amp;"""=&gt;"&amp;F10&amp;","</f>
+        <f t="shared" ref="A56:A59" si="8">""""&amp;A10&amp;"""=&gt;"&amp;F10&amp;","</f>
         <v>"Temperature"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B56" s="22"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>"Wind"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B57" s="22"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>"Batterie"=&gt;Gfx.FONT_LARGE,</v>
       </c>
       <c r="B58" s="22"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>"labelMin"=&gt;Gfx.FONT_XTINY,</v>
       </c>
       <c r="B59" s="22"/>
@@ -10705,84 +11549,84 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="str">
-        <f>""""&amp;A2&amp;"""=&gt;"&amp;G2&amp;","</f>
+        <f t="shared" ref="A63:A70" si="9">""""&amp;A2&amp;"""=&gt;"&amp;G2&amp;","</f>
         <v>"date"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B63" s="22"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="str">
-        <f>""""&amp;A3&amp;"""=&gt;"&amp;G3&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"heure"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B64" s="22"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="str">
-        <f>""""&amp;A4&amp;"""=&gt;"&amp;G4&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"notif"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B65" s="23"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="str">
-        <f>""""&amp;A5&amp;"""=&gt;"&amp;G5&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"BG"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B66" s="22"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="str">
-        <f>""""&amp;A6&amp;"""=&gt;"&amp;G6&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"Delta"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B67" s="22"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="str">
-        <f>""""&amp;A7&amp;"""=&gt;"&amp;G7&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"Elapsed"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B68" s="22"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="str">
-        <f>""""&amp;A8&amp;"""=&gt;"&amp;G8&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"ProvenanceBG"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B69" s="22"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="str">
-        <f>""""&amp;A9&amp;"""=&gt;"&amp;G9&amp;","</f>
+        <f t="shared" si="9"/>
         <v>"Secondes"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B70" s="22"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="str">
-        <f t="shared" ref="A71:A74" si="6">""""&amp;A10&amp;"""=&gt;"&amp;G10&amp;","</f>
+        <f t="shared" ref="A71:A74" si="10">""""&amp;A10&amp;"""=&gt;"&amp;G10&amp;","</f>
         <v>"Temperature"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B71" s="22"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>"Wind"=&gt;Gfx.TEXT_JUSTIFY_RIGHT,</v>
       </c>
       <c r="B72" s="22"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>"Batterie"=&gt;Gfx.TEXT_JUSTIFY_CENTER,</v>
       </c>
       <c r="B73" s="22"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>"labelMin"=&gt;Gfx.TEXT_JUSTIFY_LEFT,</v>
       </c>
       <c r="B74" s="22"/>
@@ -10822,7 +11666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -11111,7 +11955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
@@ -12120,7 +12964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>

</xml_diff>